<commit_message>
Adds more dummy data methods.
</commit_message>
<xml_diff>
--- a/user_interface/static/dummy_data/event_table.xlsx
+++ b/user_interface/static/dummy_data/event_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\CSC\MyAlmanack\user_interface\static\dummy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A6E4E4-7266-4F39-96DF-BF00A8835613}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D926500A-F0C6-4495-A45B-DCBEF3775599}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5540" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Table" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
   <si>
     <t>event_id</t>
   </si>
@@ -716,9 +716,9 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -937,7 +937,9 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G8" s="11">
         <v>1555689600000</v>
       </c>
@@ -1069,7 +1071,9 @@
       <c r="C14" s="8"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G14" s="11">
         <v>1556236800000</v>
       </c>
@@ -1333,7 +1337,9 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G26" s="11">
         <v>1555538400000</v>
       </c>
@@ -1355,7 +1361,9 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G27" s="12">
         <v>1556197200000</v>
       </c>
@@ -1817,7 +1825,9 @@
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="F48" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G48" s="13">
         <v>1556222400000</v>
       </c>
@@ -1861,7 +1871,9 @@
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="F50" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="G50" s="13">
         <v>1557237600000</v>
       </c>
@@ -2235,7 +2247,9 @@
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="F67" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G67" s="13">
         <v>1557237600000</v>
       </c>

</xml_diff>

<commit_message>
Adds more alias functionality with dummy data.
</commit_message>
<xml_diff>
--- a/user_interface/static/dummy_data/event_table.xlsx
+++ b/user_interface/static/dummy_data/event_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\CSC\MyAlmanack\user_interface\static\dummy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D926500A-F0C6-4495-A45B-DCBEF3775599}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86511E4F-8CB8-40D9-9D09-F07A9E832E60}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="5540" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2150" yWindow="3850" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Table" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
   <si>
     <t>event_id</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>eat food</t>
+  </si>
+  <si>
+    <t>XJWoEcF4qsToA0NHnKnaIlqBnfO2</t>
   </si>
 </sst>
 </file>
@@ -717,8 +720,8 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2039,7 +2042,7 @@
       </c>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" ht="14.5" thickBot="1">
+    <row r="58" spans="1:10" ht="26" thickBot="1">
       <c r="A58" s="7">
         <v>71</v>
       </c>
@@ -2059,9 +2062,11 @@
       <c r="I58" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J58" s="6"/>
-    </row>
-    <row r="59" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J58" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="26" thickBot="1">
       <c r="A59" s="7">
         <v>72</v>
       </c>
@@ -2081,9 +2086,11 @@
       <c r="I59" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J59" s="6"/>
-    </row>
-    <row r="60" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J59" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="26" thickBot="1">
       <c r="A60" s="7">
         <v>73</v>
       </c>
@@ -2103,9 +2110,11 @@
       <c r="I60" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J60" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="26" thickBot="1">
       <c r="A61" s="7">
         <v>74</v>
       </c>
@@ -2125,9 +2134,11 @@
       <c r="I61" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J61" s="6"/>
-    </row>
-    <row r="62" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J61" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="26" thickBot="1">
       <c r="A62" s="7">
         <v>75</v>
       </c>
@@ -2147,9 +2158,11 @@
       <c r="I62" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J62" s="6"/>
-    </row>
-    <row r="63" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J62" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="26" thickBot="1">
       <c r="A63" s="7">
         <v>76</v>
       </c>
@@ -2169,9 +2182,11 @@
       <c r="I63" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J63" s="6"/>
-    </row>
-    <row r="64" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J63" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="26" thickBot="1">
       <c r="A64" s="7">
         <v>77</v>
       </c>
@@ -2191,9 +2206,11 @@
       <c r="I64" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J64" s="6"/>
-    </row>
-    <row r="65" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J64" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="26" thickBot="1">
       <c r="A65" s="7">
         <v>78</v>
       </c>
@@ -2213,9 +2230,11 @@
       <c r="I65" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J65" s="6"/>
-    </row>
-    <row r="66" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J65" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="26" thickBot="1">
       <c r="A66" s="7">
         <v>79</v>
       </c>
@@ -2235,9 +2254,11 @@
       <c r="I66" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J66" s="6"/>
-    </row>
-    <row r="67" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J66" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="26" thickBot="1">
       <c r="A67" s="7">
         <v>80</v>
       </c>
@@ -2259,9 +2280,11 @@
       <c r="I67" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J67" s="6"/>
-    </row>
-    <row r="68" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J67" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="26" thickBot="1">
       <c r="A68" s="7">
         <v>81</v>
       </c>
@@ -2281,9 +2304,11 @@
       <c r="I68" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J68" s="6"/>
-    </row>
-    <row r="69" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J68" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="26" thickBot="1">
       <c r="A69" s="7">
         <v>82</v>
       </c>
@@ -2303,9 +2328,11 @@
       <c r="I69" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J69" s="6"/>
-    </row>
-    <row r="70" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J69" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="26" thickBot="1">
       <c r="A70" s="7">
         <v>83</v>
       </c>
@@ -2325,9 +2352,11 @@
       <c r="I70" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J70" s="6"/>
-    </row>
-    <row r="71" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J70" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="26" thickBot="1">
       <c r="A71" s="7">
         <v>84</v>
       </c>
@@ -2347,9 +2376,11 @@
       <c r="I71" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J71" s="6"/>
-    </row>
-    <row r="72" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J71" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="26" thickBot="1">
       <c r="A72" s="7">
         <v>85</v>
       </c>
@@ -2369,9 +2400,11 @@
       <c r="I72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J72" s="6"/>
-    </row>
-    <row r="73" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J72" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="26" thickBot="1">
       <c r="A73" s="7">
         <v>86</v>
       </c>
@@ -2391,9 +2424,11 @@
       <c r="I73" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J73" s="6"/>
-    </row>
-    <row r="74" spans="1:10" ht="14.5" thickBot="1">
+      <c r="J73" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="26" thickBot="1">
       <c r="A74" s="7">
         <v>87</v>
       </c>
@@ -2413,7 +2448,9 @@
       <c r="I74" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J74" s="6"/>
+      <c r="J74" s="6" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="75" spans="1:10" ht="12.5">
       <c r="A75" s="2"/>

</xml_diff>

<commit_message>
Adds functionality to viewing different profiles and groups. Adds Create Group modal. Fixes calendar resizing.
</commit_message>
<xml_diff>
--- a/user_interface/static/dummy_data/event_table.xlsx
+++ b/user_interface/static/dummy_data/event_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\CSC\MyAlmanack\user_interface\static\dummy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86511E4F-8CB8-40D9-9D09-F07A9E832E60}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FDA0A2-0CE8-43CE-AEF1-1A1339784502}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2150" yWindow="3850" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1810" yWindow="3510" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Table" sheetId="2" r:id="rId1"/>
@@ -244,9 +244,6 @@
     <t>dancing</t>
   </si>
   <si>
-    <t>vape</t>
-  </si>
-  <si>
     <t>Vacation</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>XJWoEcF4qsToA0NHnKnaIlqBnfO2</t>
+  </si>
+  <si>
+    <t>Vampire Movies</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2063,7 +2063,7 @@
         <v>7</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="26" thickBot="1">
@@ -2087,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="26" thickBot="1">
@@ -2095,7 +2095,7 @@
         <v>73</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -2111,7 +2111,7 @@
         <v>7</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="26" thickBot="1">
@@ -2119,7 +2119,7 @@
         <v>74</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -2135,7 +2135,7 @@
         <v>7</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="26" thickBot="1">
@@ -2143,7 +2143,7 @@
         <v>75</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
@@ -2159,7 +2159,7 @@
         <v>7</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="26" thickBot="1">
@@ -2167,7 +2167,7 @@
         <v>76</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -2183,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="26" thickBot="1">
@@ -2191,7 +2191,7 @@
         <v>77</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
@@ -2207,7 +2207,7 @@
         <v>7</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="26" thickBot="1">
@@ -2215,7 +2215,7 @@
         <v>78</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
@@ -2231,7 +2231,7 @@
         <v>7</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="26" thickBot="1">
@@ -2255,7 +2255,7 @@
         <v>7</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="26" thickBot="1">
@@ -2263,7 +2263,7 @@
         <v>80</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
@@ -2281,7 +2281,7 @@
         <v>7</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="26" thickBot="1">
@@ -2289,7 +2289,7 @@
         <v>81</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -2305,7 +2305,7 @@
         <v>7</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="26" thickBot="1">
@@ -2313,7 +2313,7 @@
         <v>82</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -2329,7 +2329,7 @@
         <v>7</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="26" thickBot="1">
@@ -2337,7 +2337,7 @@
         <v>83</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -2353,7 +2353,7 @@
         <v>7</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="26" thickBot="1">
@@ -2361,7 +2361,7 @@
         <v>84</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -2377,7 +2377,7 @@
         <v>7</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="26" thickBot="1">
@@ -2385,7 +2385,7 @@
         <v>85</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -2401,7 +2401,7 @@
         <v>7</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="26" thickBot="1">
@@ -2409,7 +2409,7 @@
         <v>86</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
@@ -2425,7 +2425,7 @@
         <v>7</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="26" thickBot="1">
@@ -2449,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="12.5">

</xml_diff>